<commit_message>
wip adding text and dialogs
</commit_message>
<xml_diff>
--- a/translation_excel.xlsx
+++ b/translation_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabri\Developer\godot-pixel-hero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D056EF13-0D6D-4B8A-9CBB-4211A86A3605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D56B4-A721-487F-A256-5CFA2434702B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2940" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{89A858D1-AEB9-4938-AB3D-89016085230C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89A858D1-AEB9-4938-AB3D-89016085230C}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
   <si>
     <t>key</t>
   </si>
@@ -43,12 +43,6 @@
     <t>OPTIONS</t>
   </si>
   <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>Opcoes</t>
-  </si>
-  <si>
     <t>LOAD_GAME</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
     <t>SWORD_DESCRIPTION</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Esta espada é uma herança dos antigos Guardiões da Luz, forjada nas chamas de um vulcão sagrado e temperada com água de um rio cristalino. Ela emite um brilho suave, lembrando os tempos de paz em xxx.</t>
   </si>
   <si>
@@ -253,9 +244,6 @@
     <t>RONAN_QUEST_2</t>
   </si>
   <si>
-    <t>Encontre Wanny na parte esquerda da Floresta Negra.</t>
-  </si>
-  <si>
     <t>RONAN_QUEST_3</t>
   </si>
   <si>
@@ -296,13 +284,147 @@
   </si>
   <si>
     <t>Você pode tambem checar o painel de Inventario pelo {start}.</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Opções</t>
+  </si>
+  <si>
+    <t>No text yet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Centuries ago, xxx flourished under the care of the benevolent Guardians of Light, led by the powerful and virtuous xxx. However, a malevolent force corrupted xxx's mind, transforming him into the Dark Lord. Betraying his fellow guardians, he plunged the realm into darkness, summoning shadowy creatures that surrounded the land.
+Despite the valiant efforts of the warriors, they couldn't halt the Dark Lord's advance. In the midst of despair, one of the guardians resisted but lost all his powers. Guided by an ancient oracle for possessing unparalleled bravery and strength to confront the now-corrupted xxx, the last guardian embarks on a solitary quest, armed with hope and courage.
+Determined to restore peace, the last guardian sets out on a lone journey, armed with hope and courage.</t>
+  </si>
+  <si>
+    <t>Séculos atrás, xxx floresceu sob os cuidados dos benevolentes Guardiões da Luz, liderados pelos poderosos e virtuosos xxx. No entanto, uma força malévola corrompeu a mente de xxx, transformando-o no Lorde das Trevas. Traindo seus companheiros guardiões, ele mergulhou o reino na escuridão, invocando criaturas sombrias que cercavam a terra.
+Apesar dos valentes esforços dos guerreiros, eles não conseguiram deter o avanço do Lorde das Trevas. Em meio ao desespero, um dos guardiões resistiu, mas perdeu todos os seus poderes. Guiado por um antigo oráculo por possuir bravura e força incomparáveis para enfrentar o agora corrompido xxx, o último guardião embarca em uma busca solitária, armado de esperança e coragem.
+Determinado a restaurar a paz, o último guardião parte em uma jornada solitária, armado com esperança e coragem.</t>
+  </si>
+  <si>
+    <t>Encontre a Wanny na parte esquerda da Floresta Sombria.</t>
+  </si>
+  <si>
+    <t>SAVE_BUTTON_TEXT</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Salvar</t>
+  </si>
+  <si>
+    <t>SOUND_TITLE</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Som</t>
+  </si>
+  <si>
+    <t>SFX_TEXT</t>
+  </si>
+  <si>
+    <t>SFX</t>
+  </si>
+  <si>
+    <t>Efeitos</t>
+  </si>
+  <si>
+    <t>MUSIC_TEXT</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Música</t>
+  </si>
+  <si>
+    <t>LANGUAGE_TITLE</t>
+  </si>
+  <si>
+    <t>Language List</t>
+  </si>
+  <si>
+    <t>LEVEL_UP_TEXT_0</t>
+  </si>
+  <si>
+    <t>Parabéns você subiu de nível!</t>
+  </si>
+  <si>
+    <t>LEVEL_UP_TEXT_1</t>
+  </si>
+  <si>
+    <t>Verifique o painel de informções do jogador no pause para aumentar seus atributos.</t>
+  </si>
+  <si>
+    <t>YOU_NEED_A_KEY_TEXT</t>
+  </si>
+  <si>
+    <t>Você precisa de uma chave.</t>
+  </si>
+  <si>
+    <t>YOU_NEED_A_WEAPON_TEXT</t>
+  </si>
+  <si>
+    <t>Você precisa de uma arma. Há muitos monstros perigosos lá.</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DIALOG_0</t>
+  </si>
+  <si>
+    <t>Eu sou o Mago do Caos!</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DIALOG_1</t>
+  </si>
+  <si>
+    <t>Sua jornada se encerra aqui, Herói.</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DIALOG_2</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_NAME</t>
+  </si>
+  <si>
+    <t>Mago do Caos</t>
+  </si>
+  <si>
+    <t>Dark Mage</t>
+  </si>
+  <si>
+    <t>Um discípulo do Lorde Das Trevas.</t>
+  </si>
+  <si>
+    <t>Agora você verá uma fração do nosso poder.</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DIALOG_3</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DEATH_DIALOG_0</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DEATH_DIALOG_1</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DEATH_DIALOG_2</t>
+  </si>
+  <si>
+    <t>DARK_MAGE_DEATH_DIALOG_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +555,26 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -779,8 +921,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1156,17 +1305,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3387B335-5F4B-44FA-9F2A-CB444B183FEA}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="200.140625" customWidth="1"/>
+    <col min="3" max="3" width="109.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,428 +1345,621 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="405" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
+      <c r="B29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>